<commit_message>
Uploaded Course Materials - Day 11.
</commit_message>
<xml_diff>
--- a/Setup and Installation/Required Software and Setup.xlsx
+++ b/Setup and Installation/Required Software and Setup.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Serial No.</t>
   </si>
@@ -74,6 +74,39 @@
     <t>https://spring.io/tools/</t>
   </si>
   <si>
+    <t>MySQL Community Server 8.0</t>
+  </si>
+  <si>
+    <t>https://dev.mysql.com/downloads/mysql/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MySQL - Setup and Installation.pptx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 'Setup and Installation' folder.</t>
+    </r>
+  </si>
+  <si>
     <t>Postman</t>
   </si>
   <si>
@@ -116,8 +149,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
@@ -188,6 +221,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -200,21 +241,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -241,14 +267,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -259,6 +277,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -266,7 +322,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,29 +330,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,13 +353,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,31 +503,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,43 +521,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,85 +533,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,6 +544,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -548,41 +596,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -593,6 +606,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,10 +633,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -635,127 +668,127 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -772,14 +805,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1108,12 +1141,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1169,15 +1202,18 @@
     <row r="6" spans="1:1">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" ht="18.75" spans="1:3">
+    <row r="7" ht="30" spans="1:4">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1187,11 +1223,11 @@
       <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -1201,11 +1237,11 @@
       <c r="A11" s="2">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -1216,10 +1252,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -1230,10 +1266,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -1243,38 +1279,42 @@
       <c r="A17" s="2">
         <v>8</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" ht="17" customHeight="1" spans="1:4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
+      <c r="C17" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75" spans="1:3">
+      <c r="A19" s="2">
+        <v>9</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" ht="18.75" spans="1:2">
+    <row r="21" ht="17" customHeight="1" spans="1:4">
+      <c r="A21" s="12"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:1">
       <c r="A22" s="2"/>
-      <c r="B22" s="13"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2"/>
     </row>
     <row r="24" ht="18.75" spans="1:2">
       <c r="A24" s="2"/>
-      <c r="B24" s="14"/>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="2"/>
+      <c r="B24" s="13"/>
     </row>
     <row r="26" ht="18.75" spans="1:2">
       <c r="A26" s="2"/>
@@ -1286,17 +1326,25 @@
     <row r="28" ht="18.75" spans="1:2">
       <c r="A28" s="2"/>
       <c r="B28" s="14"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" ht="18.75" spans="1:2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://www.oracle.com/in/java/technologies/javase/jdk11-archive-downloads.html"/>
     <hyperlink ref="C5" r:id="rId2" display="https://spring.io/tools/"/>
-    <hyperlink ref="C7" r:id="rId3" display="https://www.postman.com/downloads/"/>
-    <hyperlink ref="C9" r:id="rId4" display="https://maven.apache.org/download.cgi"/>
-    <hyperlink ref="C11" r:id="rId5" display="https://tomcat.apache.org/download-90.cgi"/>
-    <hyperlink ref="C13" r:id="rId6" display="https://www.enterprisedb.com/downloads/postgres-postgresql-downloads"/>
-    <hyperlink ref="C17" r:id="rId7" display="https://code.visualstudio.com/download"/>
-    <hyperlink ref="C15" r:id="rId8" display="https://www.pgadmin.org/download/pgadmin-4-windows/"/>
+    <hyperlink ref="C9" r:id="rId3" display="https://www.postman.com/downloads/"/>
+    <hyperlink ref="C11" r:id="rId4" display="https://maven.apache.org/download.cgi"/>
+    <hyperlink ref="C13" r:id="rId5" display="https://tomcat.apache.org/download-90.cgi"/>
+    <hyperlink ref="C15" r:id="rId6" display="https://www.enterprisedb.com/downloads/postgres-postgresql-downloads"/>
+    <hyperlink ref="C19" r:id="rId7" display="https://code.visualstudio.com/download"/>
+    <hyperlink ref="C17" r:id="rId8" display="https://www.pgadmin.org/download/pgadmin-4-windows/"/>
+    <hyperlink ref="C7" r:id="rId9" display="https://dev.mysql.com/downloads/mysql/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>